<commit_message>
Facility: remove column village_id
</commit_message>
<xml_diff>
--- a/public/facility_batch_sample.xlsx
+++ b/public/facility_batch_sample.xlsx
@@ -41,7 +41,7 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mj0uUy4wuiMoHZm7e3f7dKkDqhQOw=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mjWH9K2BG5ywJUsY6DmBoQp8z/UUg=="/>
     </ext>
   </extLst>
 </comments>
@@ -53,7 +53,7 @@
     <t>name</t>
   </si>
   <si>
-    <t>village_id</t>
+    <t>commune_id</t>
   </si>
   <si>
     <t>village_note</t>
@@ -137,10 +137,10 @@
     <t>គ្លីនិកសុខភាពឯកទេសកម្ពុជា</t>
   </si>
   <si>
-    <t>12010101</t>
+    <t>120101</t>
   </si>
   <si>
-    <t>រាជធានីភ្នំពេញ / ខណ្ឌចំការមន / សង្កាត់ទន្លេបាសាក់ / ភូមិ ១</t>
+    <t>រាជធានីភ្នំពេញ / ខណ្ឌចំការមន / សង្កាត់ទន្លេបាសាក់</t>
   </si>
   <si>
     <t>310</t>

</xml_diff>